<commit_message>
Chaged the second replicate to a biological one
</commit_message>
<xml_diff>
--- a/data/First_round_results/First Plate 050220 (Rep 3 of 3).xlsx
+++ b/data/First_round_results/First Plate 050220 (Rep 3 of 3).xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/hay278_csiro_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynbioML\data\First_round_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{7B70943E-B25F-43A8-9298-7999014A10FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C420A500-9207-42E4-B8CE-672B98971F75}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F0846C-CB21-45D1-A9F0-A07B344F644A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="1212" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{55E0826D-767D-42B2-95AC-30CE3C757662}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{55E0826D-767D-42B2-95AC-30CE3C757662}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ODGFP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -337,7 +337,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,9 +733,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:98" ht="39.6">
+    <row r="1" spans="1:98" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>5.8217592592592592E-3</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1.2766203703703703E-2</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1.9710648148148147E-2</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2.6655092592592591E-2</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3.3599537037037039E-2</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4.0543981481481479E-2</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4.7488425925925927E-2</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>5.4432870370370368E-2</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>6.1377314814814815E-2</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>6.8321759259259263E-2</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>7.5266203703703696E-2</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>8.2210648148148144E-2</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>8.9155092592592591E-2</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>9.6099537037037039E-2</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>0.10304398148148149</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:98">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>0.10998842592592593</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:98">
+    <row r="18" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>0.11693287037037037</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:98">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>0.12387731481481483</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:98">
+    <row r="20" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>0.13082175925925926</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:98">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>0.13776620370370371</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:98">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>0.14471064814814816</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:98">
+    <row r="23" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>0.15165509259259261</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:98">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>0.15859953703703702</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:98">
+    <row r="25" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>0.1655439814814815</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:98">
+    <row r="26" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>0.17248842592592592</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:98">
+    <row r="27" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>0.17943287037037037</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:98">
+    <row r="28" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>0.18637731481481482</v>
       </c>
@@ -9023,7 +9023,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:98">
+    <row r="29" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>0.19332175925925923</v>
       </c>
@@ -9319,7 +9319,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:98">
+    <row r="30" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>0.20026620370370371</v>
       </c>
@@ -9615,7 +9615,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:98">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>0.20721064814814816</v>
       </c>
@@ -9911,7 +9911,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:98">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>0.21415509259259258</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:98">
+    <row r="33" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>0.22109953703703702</v>
       </c>
@@ -10503,7 +10503,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:98">
+    <row r="34" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>0.2280439814814815</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:98">
+    <row r="35" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>0.23498842592592592</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:98">
+    <row r="36" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>0.24193287037037037</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:98">
+    <row r="37" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>0.24887731481481482</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:98">
+    <row r="38" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>0.25582175925925926</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:98">
+    <row r="39" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>0.26276620370370368</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:98">
+    <row r="40" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>0.26971064814814816</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:98">
+    <row r="41" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>0.27665509259259258</v>
       </c>
@@ -12871,7 +12871,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:98">
+    <row r="42" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>0.28359953703703705</v>
       </c>
@@ -13167,7 +13167,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:98">
+    <row r="43" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>0.29054398148148147</v>
       </c>
@@ -13463,7 +13463,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:98">
+    <row r="44" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>0.29748842592592589</v>
       </c>
@@ -13759,7 +13759,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:98">
+    <row r="45" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>0.30443287037037037</v>
       </c>
@@ -14055,7 +14055,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:98">
+    <row r="46" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>0.31137731481481484</v>
       </c>
@@ -14351,7 +14351,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:98">
+    <row r="47" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>0.31832175925925926</v>
       </c>
@@ -14647,7 +14647,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:98">
+    <row r="48" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>0.32526620370370368</v>
       </c>
@@ -14943,7 +14943,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:98">
+    <row r="49" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>0.33221064814814816</v>
       </c>
@@ -15239,7 +15239,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:98">
+    <row r="50" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>0.33915509259259258</v>
       </c>
@@ -15535,7 +15535,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:98" ht="39.6">
+    <row r="52" spans="1:98" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -15831,7 +15831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:98">
+    <row r="53" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>6.6550925925925935E-3</v>
       </c>
@@ -16127,7 +16127,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:98">
+    <row r="54" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>1.3599537037037037E-2</v>
       </c>
@@ -16423,7 +16423,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:98">
+    <row r="55" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2.0543981481481479E-2</v>
       </c>
@@ -16719,7 +16719,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:98">
+    <row r="56" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2.7488425925925927E-2</v>
       </c>
@@ -17015,7 +17015,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:98">
+    <row r="57" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>3.4432870370370371E-2</v>
       </c>
@@ -17311,7 +17311,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:98">
+    <row r="58" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>4.1377314814814818E-2</v>
       </c>
@@ -17607,7 +17607,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="59" spans="1:98">
+    <row r="59" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>4.8321759259259266E-2</v>
       </c>
@@ -17903,7 +17903,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:98">
+    <row r="60" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>5.5266203703703699E-2</v>
       </c>
@@ -18199,7 +18199,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:98">
+    <row r="61" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>6.2210648148148147E-2</v>
       </c>
@@ -18495,7 +18495,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:98">
+    <row r="62" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>6.9155092592592601E-2</v>
       </c>
@@ -18791,7 +18791,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="63" spans="1:98">
+    <row r="63" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>7.6099537037037035E-2</v>
       </c>
@@ -19087,7 +19087,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:98">
+    <row r="64" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>8.3043981481481483E-2</v>
       </c>
@@ -19383,7 +19383,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:98">
+    <row r="65" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>8.998842592592593E-2</v>
       </c>
@@ -19679,7 +19679,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="1:98">
+    <row r="66" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>9.6932870370370364E-2</v>
       </c>
@@ -19975,7 +19975,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:98">
+    <row r="67" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>0.10387731481481481</v>
       </c>
@@ -20271,7 +20271,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:98">
+    <row r="68" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>0.11082175925925926</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="69" spans="1:98">
+    <row r="69" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>0.11776620370370371</v>
       </c>
@@ -20863,7 +20863,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="70" spans="1:98">
+    <row r="70" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>0.12471064814814814</v>
       </c>
@@ -21159,7 +21159,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:98">
+    <row r="71" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>0.13165509259259259</v>
       </c>
@@ -21455,7 +21455,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:98">
+    <row r="72" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>0.13859953703703703</v>
       </c>
@@ -21751,7 +21751,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="73" spans="1:98">
+    <row r="73" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>0.14554398148148148</v>
       </c>
@@ -22047,7 +22047,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:98">
+    <row r="74" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>0.15248842592592593</v>
       </c>
@@ -22343,7 +22343,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:98">
+    <row r="75" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>0.15943287037037038</v>
       </c>
@@ -22639,7 +22639,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="76" spans="1:98">
+    <row r="76" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>0.1663773148148148</v>
       </c>
@@ -22935,7 +22935,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:98">
+    <row r="77" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>0.17332175925925927</v>
       </c>
@@ -23231,7 +23231,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:98">
+    <row r="78" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>0.18026620370370372</v>
       </c>
@@ -23527,7 +23527,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:98">
+    <row r="79" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>0.18721064814814814</v>
       </c>
@@ -23823,7 +23823,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="80" spans="1:98">
+    <row r="80" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>0.19415509259259259</v>
       </c>
@@ -24119,7 +24119,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="81" spans="1:98">
+    <row r="81" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>0.20109953703703706</v>
       </c>
@@ -24415,7 +24415,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="82" spans="1:98">
+    <row r="82" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>0.20804398148148148</v>
       </c>
@@ -24711,7 +24711,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="83" spans="1:98">
+    <row r="83" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>0.21498842592592593</v>
       </c>
@@ -25007,7 +25007,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="84" spans="1:98">
+    <row r="84" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>0.22193287037037038</v>
       </c>
@@ -25303,7 +25303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="85" spans="1:98">
+    <row r="85" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>0.2288773148148148</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:98">
+    <row r="86" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>0.23582175925925927</v>
       </c>
@@ -25895,7 +25895,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="87" spans="1:98">
+    <row r="87" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>0.24276620370370372</v>
       </c>
@@ -26191,7 +26191,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:98">
+    <row r="88" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>0.24971064814814814</v>
       </c>
@@ -26487,7 +26487,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="89" spans="1:98">
+    <row r="89" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>0.25665509259259262</v>
       </c>
@@ -26783,7 +26783,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:98">
+    <row r="90" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>0.26359953703703703</v>
       </c>
@@ -27079,7 +27079,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="91" spans="1:98">
+    <row r="91" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>0.27054398148148145</v>
       </c>
@@ -27375,7 +27375,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="92" spans="1:98">
+    <row r="92" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>0.27748842592592593</v>
       </c>
@@ -27671,7 +27671,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:98">
+    <row r="93" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>0.28443287037037041</v>
       </c>
@@ -27967,7 +27967,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="1:98">
+    <row r="94" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>0.29137731481481483</v>
       </c>
@@ -28263,7 +28263,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="95" spans="1:98">
+    <row r="95" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>0.29832175925925924</v>
       </c>
@@ -28559,7 +28559,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="96" spans="1:98">
+    <row r="96" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>0.30526620370370372</v>
       </c>
@@ -28855,7 +28855,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:98">
+    <row r="97" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>0.31221064814814814</v>
       </c>
@@ -29151,7 +29151,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="98" spans="1:98">
+    <row r="98" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>0.31915509259259262</v>
       </c>
@@ -29447,7 +29447,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="99" spans="1:98">
+    <row r="99" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>0.32609953703703703</v>
       </c>
@@ -29743,7 +29743,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="100" spans="1:98">
+    <row r="100" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>0.33304398148148145</v>
       </c>
@@ -30039,7 +30039,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="101" spans="1:98">
+    <row r="101" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>0.33998842592592587</v>
       </c>
@@ -30346,12 +30346,12 @@
   <dimension ref="A1:CL50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A50"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:90">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -30623,7 +30623,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:90">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -30984,7 +30984,7 @@
         <v>1161.2903225806451</v>
       </c>
     </row>
-    <row r="3" spans="1:90">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -31345,7 +31345,7 @@
         <v>1023.0769230769231</v>
       </c>
     </row>
-    <row r="4" spans="1:90">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>20</v>
       </c>
@@ -31706,7 +31706,7 @@
         <v>964.02877697841723</v>
       </c>
     </row>
-    <row r="5" spans="1:90">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>30</v>
       </c>
@@ -32067,7 +32067,7 @@
         <v>920.5298013245033</v>
       </c>
     </row>
-    <row r="6" spans="1:90">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>40</v>
       </c>
@@ -32428,7 +32428,7 @@
         <v>753.01204819277109</v>
       </c>
     </row>
-    <row r="7" spans="1:90">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>50</v>
       </c>
@@ -32789,7 +32789,7 @@
         <v>706.52173913043475</v>
       </c>
     </row>
-    <row r="8" spans="1:90">
+    <row r="8" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>60</v>
       </c>
@@ -33150,7 +33150,7 @@
         <v>699.50738916256148</v>
       </c>
     </row>
-    <row r="9" spans="1:90">
+    <row r="9" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>70</v>
       </c>
@@ -33511,7 +33511,7 @@
         <v>553.57142857142856</v>
       </c>
     </row>
-    <row r="10" spans="1:90">
+    <row r="10" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>80</v>
       </c>
@@ -33872,7 +33872,7 @@
         <v>540.98360655737702</v>
       </c>
     </row>
-    <row r="11" spans="1:90">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>90</v>
       </c>
@@ -34233,7 +34233,7 @@
         <v>475.47169811320754</v>
       </c>
     </row>
-    <row r="12" spans="1:90">
+    <row r="12" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>100</v>
       </c>
@@ -34594,7 +34594,7 @@
         <v>405.5944055944056</v>
       </c>
     </row>
-    <row r="13" spans="1:90">
+    <row r="13" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>110</v>
       </c>
@@ -34955,7 +34955,7 @@
         <v>402.59740259740261</v>
       </c>
     </row>
-    <row r="14" spans="1:90">
+    <row r="14" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>120</v>
       </c>
@@ -35316,7 +35316,7 @@
         <v>422.01834862385317</v>
       </c>
     </row>
-    <row r="15" spans="1:90">
+    <row r="15" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>130</v>
       </c>
@@ -35677,7 +35677,7 @@
         <v>367.52136752136755</v>
       </c>
     </row>
-    <row r="16" spans="1:90">
+    <row r="16" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>140</v>
       </c>
@@ -36038,7 +36038,7 @@
         <v>344.17344173441734</v>
       </c>
     </row>
-    <row r="17" spans="1:90">
+    <row r="17" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>150</v>
       </c>
@@ -36399,7 +36399,7 @@
         <v>356.77083333333331</v>
       </c>
     </row>
-    <row r="18" spans="1:90">
+    <row r="18" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>160</v>
       </c>
@@ -36760,7 +36760,7 @@
         <v>361.11111111111109</v>
       </c>
     </row>
-    <row r="19" spans="1:90">
+    <row r="19" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>170</v>
       </c>
@@ -37121,7 +37121,7 @@
         <v>349.51456310679612</v>
       </c>
     </row>
-    <row r="20" spans="1:90">
+    <row r="20" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>180</v>
       </c>
@@ -37482,7 +37482,7 @@
         <v>327.83018867924528</v>
       </c>
     </row>
-    <row r="21" spans="1:90">
+    <row r="21" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>190</v>
       </c>
@@ -37843,7 +37843,7 @@
         <v>347.03196347031962</v>
       </c>
     </row>
-    <row r="22" spans="1:90">
+    <row r="22" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>200</v>
       </c>
@@ -38204,7 +38204,7 @@
         <v>334.83146067415731</v>
       </c>
     </row>
-    <row r="23" spans="1:90">
+    <row r="23" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>210</v>
       </c>
@@ -38565,7 +38565,7 @@
         <v>353.84615384615381</v>
       </c>
     </row>
-    <row r="24" spans="1:90">
+    <row r="24" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>220</v>
       </c>
@@ -38926,7 +38926,7 @@
         <v>355.60344827586204</v>
       </c>
     </row>
-    <row r="25" spans="1:90">
+    <row r="25" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>230</v>
       </c>
@@ -39287,7 +39287,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="26" spans="1:90">
+    <row r="26" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>240</v>
       </c>
@@ -39648,7 +39648,7 @@
         <v>329.2433537832311</v>
       </c>
     </row>
-    <row r="27" spans="1:90">
+    <row r="27" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>250</v>
       </c>
@@ -40009,7 +40009,7 @@
         <v>349.90059642147116</v>
       </c>
     </row>
-    <row r="28" spans="1:90">
+    <row r="28" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>260</v>
       </c>
@@ -40370,7 +40370,7 @@
         <v>352.14007782101169</v>
       </c>
     </row>
-    <row r="29" spans="1:90">
+    <row r="29" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>270</v>
       </c>
@@ -40731,7 +40731,7 @@
         <v>336.53846153846155</v>
       </c>
     </row>
-    <row r="30" spans="1:90">
+    <row r="30" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>280</v>
       </c>
@@ -41092,7 +41092,7 @@
         <v>344.10646387832696</v>
       </c>
     </row>
-    <row r="31" spans="1:90">
+    <row r="31" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>290</v>
       </c>
@@ -41453,7 +41453,7 @@
         <v>360.377358490566</v>
       </c>
     </row>
-    <row r="32" spans="1:90">
+    <row r="32" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>300</v>
       </c>
@@ -41814,7 +41814,7 @@
         <v>356.34328358208955</v>
       </c>
     </row>
-    <row r="33" spans="1:90">
+    <row r="33" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>310</v>
       </c>
@@ -42175,7 +42175,7 @@
         <v>374.77148080438752</v>
       </c>
     </row>
-    <row r="34" spans="1:90">
+    <row r="34" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>320</v>
       </c>
@@ -42536,7 +42536,7 @@
         <v>391.30434782608694</v>
       </c>
     </row>
-    <row r="35" spans="1:90">
+    <row r="35" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>330</v>
       </c>
@@ -42897,7 +42897,7 @@
         <v>369.56521739130432</v>
       </c>
     </row>
-    <row r="36" spans="1:90">
+    <row r="36" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>340</v>
       </c>
@@ -43258,7 +43258,7 @@
         <v>389.18918918918916</v>
       </c>
     </row>
-    <row r="37" spans="1:90">
+    <row r="37" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>350</v>
       </c>
@@ -43619,7 +43619,7 @@
         <v>379.24865831842573</v>
       </c>
     </row>
-    <row r="38" spans="1:90">
+    <row r="38" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>360</v>
       </c>
@@ -43980,7 +43980,7 @@
         <v>387.49999999999994</v>
       </c>
     </row>
-    <row r="39" spans="1:90">
+    <row r="39" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>370</v>
       </c>
@@ -44341,7 +44341,7 @@
         <v>404.29338103756703</v>
       </c>
     </row>
-    <row r="40" spans="1:90">
+    <row r="40" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>380</v>
       </c>
@@ -44702,7 +44702,7 @@
         <v>383.24420677361849</v>
       </c>
     </row>
-    <row r="41" spans="1:90">
+    <row r="41" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>390</v>
       </c>
@@ -45063,7 +45063,7 @@
         <v>390.76376554174072</v>
       </c>
     </row>
-    <row r="42" spans="1:90">
+    <row r="42" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>400</v>
       </c>
@@ -45424,7 +45424,7 @@
         <v>406.4171122994652</v>
       </c>
     </row>
-    <row r="43" spans="1:90">
+    <row r="43" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>410</v>
       </c>
@@ -45785,7 +45785,7 @@
         <v>399.64476021314391</v>
       </c>
     </row>
-    <row r="44" spans="1:90">
+    <row r="44" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>420</v>
       </c>
@@ -46146,7 +46146,7 @@
         <v>396.82539682539687</v>
       </c>
     </row>
-    <row r="45" spans="1:90">
+    <row r="45" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>430</v>
       </c>
@@ -46507,7 +46507,7 @@
         <v>417.83216783216784</v>
       </c>
     </row>
-    <row r="46" spans="1:90">
+    <row r="46" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>440</v>
       </c>
@@ -46868,7 +46868,7 @@
         <v>417.54385964912285</v>
       </c>
     </row>
-    <row r="47" spans="1:90">
+    <row r="47" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>450</v>
       </c>
@@ -47229,7 +47229,7 @@
         <v>423.55008787346225</v>
       </c>
     </row>
-    <row r="48" spans="1:90">
+    <row r="48" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>460</v>
       </c>
@@ -47590,7 +47590,7 @@
         <v>423.61111111111114</v>
       </c>
     </row>
-    <row r="49" spans="1:90">
+    <row r="49" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>470</v>
       </c>
@@ -47951,7 +47951,7 @@
         <v>447.73519163763069</v>
       </c>
     </row>
-    <row r="50" spans="1:90">
+    <row r="50" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>480</v>
       </c>
@@ -48318,6 +48318,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="ebbfb97d-8400-4246-978d-8b68e4a1ec72">2J45DRNPYS3J-2128470947-29</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="ebbfb97d-8400-4246-978d-8b68e4a1ec72">
+      <Url>https://csiroau.sharepoint.com/sites/SOLARIS/_layouts/15/DocIdRedir.aspx?ID=2J45DRNPYS3J-2128470947-29</Url>
+      <Description>2J45DRNPYS3J-2128470947-29</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005C35F8E5208B414AB6002F6CEC7B4BF2" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="142c79e7eb87feefba26b8692b85b6e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98fdb299-815b-4672-8b02-d1d8c19b8436" xmlns:ns3="ebbfb97d-8400-4246-978d-8b68e4a1ec72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="800c5b84226e565e3cfc0ce8f4b34bf7" ns2:_="" ns3:_="">
     <xsd:import namespace="98fdb299-815b-4672-8b02-d1d8c19b8436"/>
@@ -48479,89 +48550,47 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="ebbfb97d-8400-4246-978d-8b68e4a1ec72">2J45DRNPYS3J-2128470947-29</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="ebbfb97d-8400-4246-978d-8b68e4a1ec72">
-      <Url>https://csiroau.sharepoint.com/sites/SOLARIS/_layouts/15/DocIdRedir.aspx?ID=2J45DRNPYS3J-2128470947-29</Url>
-      <Description>2J45DRNPYS3J-2128470947-29</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B619803C-BE31-4D84-B9F4-2BA948C37A66}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36D034EC-2F5E-4C5F-ACCE-1BD7AFBA36F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6473668C-30BE-4BC4-8531-BE7B70D0B8FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27BB7132-DDFF-4BEE-BD89-AE0FC4927ED9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ebbfb97d-8400-4246-978d-8b68e4a1ec72"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27BB7132-DDFF-4BEE-BD89-AE0FC4927ED9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6473668C-30BE-4BC4-8531-BE7B70D0B8FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36D034EC-2F5E-4C5F-ACCE-1BD7AFBA36F8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B619803C-BE31-4D84-B9F4-2BA948C37A66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="98fdb299-815b-4672-8b02-d1d8c19b8436"/>
+    <ds:schemaRef ds:uri="ebbfb97d-8400-4246-978d-8b68e4a1ec72"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>